<commit_message>
Lesson 7 Dialogue ANglic
</commit_message>
<xml_diff>
--- a/Zdetl Lexicon.xlsx
+++ b/Zdetl Lexicon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkaz1\Documents\GitHub\Zdetl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC9A43-1580-4499-8758-B3AC1E8C3D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE9F1B1-2937-4DE8-B9F1-95DEBE2D7005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="891" activeTab="6" xr2:uid="{06097C92-1E44-4EB6-8222-C9DA7786637A}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5770" uniqueCount="3142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5806" uniqueCount="3166">
   <si>
     <t>Zhdetl word</t>
   </si>
@@ -9512,6 +9512,78 @@
   </si>
   <si>
     <t>raincoat</t>
+  </si>
+  <si>
+    <t>puddle</t>
+  </si>
+  <si>
+    <t>akala</t>
+  </si>
+  <si>
+    <t>pool</t>
+  </si>
+  <si>
+    <t>rintakala</t>
+  </si>
+  <si>
+    <t>RINTAKALA</t>
+  </si>
+  <si>
+    <t>AKALA</t>
+  </si>
+  <si>
+    <t>to splash</t>
+  </si>
+  <si>
+    <t>chikiatse'</t>
+  </si>
+  <si>
+    <t>ĈIKĨṮE'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chikiats </t>
+  </si>
+  <si>
+    <t>ĈIKĨṮ</t>
+  </si>
+  <si>
+    <t>splash</t>
+  </si>
+  <si>
+    <t>kliazheze'</t>
+  </si>
+  <si>
+    <t>ḰĨŹEZE'</t>
+  </si>
+  <si>
+    <t>to make wet</t>
+  </si>
+  <si>
+    <t>kliazheve'</t>
+  </si>
+  <si>
+    <t>ḰĨŹEVE'</t>
+  </si>
+  <si>
+    <t>to become wet</t>
+  </si>
+  <si>
+    <t>a Zhodani "pigeon"</t>
+  </si>
+  <si>
+    <t>chilotl</t>
+  </si>
+  <si>
+    <t>ĈILOṪ</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>atlotl</t>
+  </si>
+  <si>
+    <t>AṪOṪ</t>
   </si>
 </sst>
 </file>
@@ -9901,10 +9973,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9920,6 +9992,16 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -10000,16 +10082,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -11932,8 +12004,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4039E8B-8AC1-44D4-939F-61521D537543}" name="Zhdetl" displayName="Zhdetl" ref="A1:B186" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B186" xr:uid="{B2E9EE69-E126-4FC1-ACEF-C598B63AECDE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5FF4A609-EB29-4591-80AA-89AF1E219E8F}" uniqueName="1" name="Word" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{7D4C4436-96EC-4C21-A85D-7C6AE2F8E895}" uniqueName="2" name="Meaning" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{5FF4A609-EB29-4591-80AA-89AF1E219E8F}" uniqueName="1" name="Word" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7D4C4436-96EC-4C21-A85D-7C6AE2F8E895}" uniqueName="2" name="Meaning" queryTableFieldId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12239,8 +12311,8 @@
   <dimension ref="A1:D751"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A444" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D460" sqref="D460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -18663,7 +18735,7 @@
         <v>1068</v>
       </c>
       <c r="D459" s="12" t="s">
-        <v>327</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.3">
@@ -24563,15 +24635,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>947</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -27778,7 +27850,7 @@
     <sortCondition ref="A2:A119"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D33" location="'Zhdetl (from Alien Book 4)'!A19" display="'Zhdetl (from Alien Book 4)'!A19" xr:uid="{F22ED44C-2884-447F-9EEA-635AD96A4C7F}"/>
@@ -32278,8 +32350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F72B619-F07E-4E67-B084-4F94FC5DF445}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32896,7 +32968,7 @@
       <c r="A44" t="s">
         <v>817</v>
       </c>
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="91" t="s">
         <v>1600</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -32935,57 +33007,156 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="83"/>
+      <c r="A47" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B47" s="83" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3142</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="83"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="83"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="83"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="83"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="83"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="83"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="83"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="83"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>3143</v>
+      </c>
+      <c r="B48" s="83" t="s">
+        <v>3147</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B49" s="83" t="s">
+        <v>3150</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B50" s="83" t="s">
+        <v>3152</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B51" s="83" t="s">
+        <v>3155</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B52" s="83" t="s">
+        <v>3158</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="83" t="s">
+        <v>2264</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>3161</v>
+      </c>
+      <c r="B54" s="83" t="s">
+        <v>3162</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B55" s="83" t="s">
+        <v>3165</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B56" s="83"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" s="83"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" s="83"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" s="83"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" s="83"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" s="83"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" s="83"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" s="83"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64" s="83"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
@@ -33197,28 +33368,28 @@
     <cfRule type="duplicateValues" dxfId="14" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -34169,13 +34340,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A8 A10">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A8 A10">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B13">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>